<commit_message>
Data needs to added to the Excel File for Game, Characters and Costumes (?)
</commit_message>
<xml_diff>
--- a/SuperSmashData.xlsx
+++ b/SuperSmashData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scottjm1\git\SuperSmashBrothersDatabaseFrontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429C3BAA-9839-4D38-BCAE-A3353AC29747}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9017C1EB-E020-495A-B5C4-5645E37ABC94}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" activeTab="3" xr2:uid="{B432F1D2-921E-4BEB-BE4A-1CBA209F3298}"/>
   </bookViews>
@@ -16,9 +16,8 @@
     <sheet name="Game Data" sheetId="3" r:id="rId1"/>
     <sheet name="Character Data" sheetId="4" r:id="rId2"/>
     <sheet name="Costume Data" sheetId="5" r:id="rId3"/>
-    <sheet name="Move Data" sheetId="6" r:id="rId4"/>
+    <sheet name="Stage Data" sheetId="1" r:id="rId4"/>
     <sheet name="Item Data" sheetId="2" r:id="rId5"/>
-    <sheet name="Stage Data" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -560,13 +559,176 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3504853D-76B8-410B-849F-01B41F6B5793}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69CF2EBC-9D7C-4FFA-8418-B2473107AF8E}">
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -675,179 +837,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69CF2EBC-9D7C-4FFA-8418-B2473107AF8E}">
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
changed moves in importer
</commit_message>
<xml_diff>
--- a/SuperSmashData.xlsx
+++ b/SuperSmashData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lakempca\git\SuperSmashBrothersDatabaseFrontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5926EC-DA2E-4ACB-987A-2CD09ECBF319}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BF2FCA-5B32-4A71-ADE8-092AC6B3C8C6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="17256" windowHeight="5652" activeTab="2" xr2:uid="{B432F1D2-921E-4BEB-BE4A-1CBA209F3298}"/>
+    <workbookView xWindow="0" yWindow="912" windowWidth="17256" windowHeight="5652" activeTab="2" xr2:uid="{B432F1D2-921E-4BEB-BE4A-1CBA209F3298}"/>
   </bookViews>
   <sheets>
     <sheet name="Game Data" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -176,6 +176,21 @@
   </si>
   <si>
     <t>MoveID</t>
+  </si>
+  <si>
+    <t>smash</t>
+  </si>
+  <si>
+    <t>special</t>
+  </si>
+  <si>
+    <t>strong</t>
+  </si>
+  <si>
+    <t>up</t>
+  </si>
+  <si>
+    <t>down</t>
   </si>
 </sst>
 </file>
@@ -729,21 +744,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BCE0B50-79ED-474D-BBDD-52FBDF88450F}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.21875" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
     <col min="5" max="5" width="19.88671875" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>44</v>
       </c>
@@ -765,22 +782,19 @@
       <c r="G1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -791,68 +805,74 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>13</v>
+      </c>
       <c r="G3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4">
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <v>11</v>
+      </c>
       <c r="G4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
       <c r="G5">
         <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G14">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed data import for all tables and added database creation script
</commit_message>
<xml_diff>
--- a/SuperSmashData.xlsx
+++ b/SuperSmashData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scottjm1\git\SuperSmashBrothersDatabaseFrontend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lakempca\git\SuperSmashBrothersDatabaseFrontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DF6116-5946-473D-8480-C7FC131C0922}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430A14BF-0EEF-402F-B42B-F1D8634DAE6D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1824" windowWidth="17256" windowHeight="5652" activeTab="2" xr2:uid="{B432F1D2-921E-4BEB-BE4A-1CBA209F3298}"/>
+    <workbookView xWindow="0" yWindow="6840" windowWidth="17256" windowHeight="5652" activeTab="6" xr2:uid="{B432F1D2-921E-4BEB-BE4A-1CBA209F3298}"/>
   </bookViews>
   <sheets>
     <sheet name="Game Data" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Move Sheet" sheetId="6" r:id="rId3"/>
     <sheet name="Stage Data" sheetId="1" r:id="rId4"/>
     <sheet name="Item Data" sheetId="2" r:id="rId5"/>
+    <sheet name="User" sheetId="8" r:id="rId6"/>
+    <sheet name="UserFavorites" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -188,6 +190,48 @@
   </si>
   <si>
     <t>down</t>
+  </si>
+  <si>
+    <t>Super Mario Bros</t>
+  </si>
+  <si>
+    <t>Bowser</t>
+  </si>
+  <si>
+    <t>Peach</t>
+  </si>
+  <si>
+    <t>Duck Hunt</t>
+  </si>
+  <si>
+    <t>Hammer</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>mayor</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>team</t>
+  </si>
+  <si>
+    <t>answer</t>
+  </si>
+  <si>
+    <t>here</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t>Character</t>
   </si>
 </sst>
 </file>
@@ -597,7 +641,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -691,10 +735,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52AB7372-A1C1-4846-A172-B79558291421}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -736,6 +780,142 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3">
+        <v>18</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4">
+        <v>19</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7">
+        <v>18</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8">
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -743,10 +923,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BCE0B50-79ED-474D-BBDD-52FBDF88450F}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -801,7 +981,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -821,7 +1001,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -841,22 +1021,102 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
         <v>52</v>
       </c>
       <c r="E5" s="6">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F5" s="6">
-        <v>5</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="6">
+        <v>10</v>
+      </c>
+      <c r="F6" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="6">
+        <v>12</v>
+      </c>
+      <c r="F7" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="6">
+        <v>9</v>
+      </c>
+      <c r="F8" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="6">
+        <v>9</v>
+      </c>
+      <c r="F9" s="6">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -866,10 +1126,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69CF2EBC-9D7C-4FFA-8418-B2473107AF8E}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A12" sqref="A12:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1034,6 +1294,20 @@
         <v>18</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1041,10 +1315,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D11CEFC-C847-4111-BEE4-751C9D330C23}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1139,8 +1413,121 @@
         <v>18</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4279F10D-64D5-4A03-A4A9-152212DA002D}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A0A3E6-6CC4-4607-9AA8-B515EB9D346F}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>